<commit_message>
minor changes to SAM
</commit_message>
<xml_diff>
--- a/Data/Raw data/NN_SAM_2020.xlsx
+++ b/Data/Raw data/NN_SAM_2020.xlsx
@@ -507,10 +507,10 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="56.7"/>
   </cols>
@@ -851,14 +851,14 @@
   <dimension ref="A1:AZ52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="T25" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="X1" activeCellId="0" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AZ23" activeCellId="0" sqref="AZ23"/>
+      <selection pane="topRight" activeCell="T1" activeCellId="0" sqref="T1"/>
+      <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="AR48" activeCellId="0" sqref="AR48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.71"/>
   </cols>
@@ -1704,7 +1704,7 @@
         <v>70</v>
       </c>
       <c r="E44" s="0" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F44" s="0" t="n">
         <v>45</v>
@@ -1719,7 +1719,7 @@
         <v>50</v>
       </c>
       <c r="J44" s="0" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="K44" s="0" t="n">
         <v>55</v>
@@ -1780,7 +1780,7 @@
         <v>60</v>
       </c>
       <c r="E45" s="0" t="n">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F45" s="0" t="n">
         <v>60</v>
@@ -1795,7 +1795,7 @@
         <v>70</v>
       </c>
       <c r="J45" s="0" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="K45" s="0" t="n">
         <v>45</v>
@@ -1847,7 +1847,7 @@
         <v>1715</v>
       </c>
       <c r="AR46" s="0" t="n">
-        <v>240</v>
+        <v>100</v>
       </c>
       <c r="AS46" s="0" t="n">
         <v>80</v>
@@ -1862,7 +1862,7 @@
         <v>30</v>
       </c>
       <c r="AR47" s="0" t="n">
-        <v>280</v>
+        <v>120</v>
       </c>
       <c r="AS47" s="0" t="n">
         <v>110</v>
@@ -1877,7 +1877,7 @@
         <v>32</v>
       </c>
       <c r="AR48" s="0" t="n">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="AS48" s="0" t="n">
         <v>155</v>
@@ -1892,7 +1892,7 @@
         <v>36</v>
       </c>
       <c r="AR49" s="0" t="n">
-        <v>60</v>
+        <v>190</v>
       </c>
       <c r="AS49" s="0" t="n">
         <v>210</v>
@@ -1907,7 +1907,7 @@
         <v>40</v>
       </c>
       <c r="AR50" s="0" t="n">
-        <v>50</v>
+        <v>270</v>
       </c>
       <c r="AS50" s="0" t="n">
         <v>330</v>

</xml_diff>

<commit_message>
model.py sends tables straight to sql db (6th positional argument for model.py is now database name), also adjusted endowments
</commit_message>
<xml_diff>
--- a/Data/Raw data/NN_SAM_2020.xlsx
+++ b/Data/Raw data/NN_SAM_2020.xlsx
@@ -507,10 +507,10 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="56.7"/>
   </cols>
@@ -855,10 +855,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="T1" activeCellId="0" sqref="T1"/>
       <selection pane="bottomLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="AR48" activeCellId="0" sqref="AR48"/>
+      <selection pane="bottomRight" activeCell="AR51" activeCellId="0" sqref="AR51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.71"/>
   </cols>
@@ -1850,7 +1850,7 @@
         <v>85</v>
       </c>
       <c r="AS46" s="0" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1858,10 +1858,10 @@
         <v>30</v>
       </c>
       <c r="AR47" s="0" t="n">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="AS47" s="0" t="n">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1869,10 +1869,10 @@
         <v>32</v>
       </c>
       <c r="AR48" s="0" t="n">
+        <v>125</v>
+      </c>
+      <c r="AS48" s="0" t="n">
         <v>130</v>
-      </c>
-      <c r="AS48" s="0" t="n">
-        <v>155</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1880,10 +1880,10 @@
         <v>36</v>
       </c>
       <c r="AR49" s="0" t="n">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="AS49" s="0" t="n">
-        <v>210</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1891,10 +1891,10 @@
         <v>40</v>
       </c>
       <c r="AR50" s="0" t="n">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="AS50" s="0" t="n">
-        <v>330</v>
+        <v>385</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>